<commit_message>
fichier bien généré et fonctionnel
</commit_message>
<xml_diff>
--- a/Excels ressources/FicheProf.xlsx
+++ b/Excels ressources/FicheProf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maily\PycharmProjects\SAE_pycharm\Excels ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3F300B-965A-4CB1-A982-15223A23C1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE205E0-BBFF-4448-9C19-1DF8534F1632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="1785" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exemple" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Fiche Professeur</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Interventions</t>
   </si>
   <si>
-    <t>Matières</t>
-  </si>
-  <si>
     <t>CM</t>
   </si>
   <si>
@@ -62,17 +59,26 @@
     <t>TP non dedoubles</t>
   </si>
   <si>
-    <t>Tests</t>
-  </si>
-  <si>
     <t>Volumes horaires</t>
+  </si>
+  <si>
+    <t>Matieres</t>
+  </si>
+  <si>
+    <t>BUT1/BUT2/BUT3</t>
+  </si>
+  <si>
+    <t>Total en HETD</t>
+  </si>
+  <si>
+    <t>TP à déclarer ARES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,16 +86,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -97,12 +125,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,63 +507,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="1" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
+      <c r="G10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>